<commit_message>
Correção nos dados de temperatura do município de Curralinho
</commit_message>
<xml_diff>
--- a/data/dataset.xlsx
+++ b/data/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://techleadit-my.sharepoint.com/personal/jailson_filho_techlead_com_br/Documents/Área de Trabalho/mestrado/main-mestrado/2. doing/7_repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{72833F69-BC0F-4973-995B-A1CC3DB87F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28C1D17F-9CD6-4047-A645-B9D21B6BE5C9}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{72833F69-BC0F-4973-995B-A1CC3DB87F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8035FB9F-7E5E-4215-BC61-D0072D3AFB90}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,10 +1031,10 @@
   <dimension ref="A1:V1008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D281" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="J293" sqref="J293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20016,7 +20016,7 @@
         <v>3181.1049522888211</v>
       </c>
       <c r="M296" s="18">
-        <v>0</v>
+        <v>27.710000000000036</v>
       </c>
       <c r="N296" s="10">
         <v>31591</v>
@@ -20072,7 +20072,7 @@
         <v>4866.5943960510267</v>
       </c>
       <c r="M297" s="18">
-        <v>0</v>
+        <v>28.29000000000002</v>
       </c>
       <c r="N297" s="10">
         <v>32248</v>
@@ -20128,7 +20128,7 @@
         <v>2159.5666572448549</v>
       </c>
       <c r="M298" s="18">
-        <v>0</v>
+        <v>27.650000000000034</v>
       </c>
       <c r="N298" s="10">
         <v>32881</v>
@@ -20196,7 +20196,7 @@
         <v>3589.5563142333895</v>
       </c>
       <c r="M299" s="18">
-        <v>0</v>
+        <v>27.430000000000007</v>
       </c>
       <c r="N299" s="10">
         <v>33490</v>
@@ -20264,7 +20264,7 @@
         <v>690.39417982175917</v>
       </c>
       <c r="M300" s="18">
-        <v>0</v>
+        <v>26.950000000000045</v>
       </c>
       <c r="N300" s="10">
         <v>33893</v>
@@ -20332,7 +20332,7 @@
         <v>2301.9021371521271</v>
       </c>
       <c r="M301" s="18">
-        <v>0</v>
+        <v>26.850000000000023</v>
       </c>
       <c r="N301" s="10">
         <v>34448</v>
@@ -20397,7 +20397,7 @@
         <v>3575.7336941160688</v>
       </c>
       <c r="M302" s="18">
-        <v>0</v>
+        <v>28.150000000000034</v>
       </c>
       <c r="N302" s="10">
         <v>34994</v>

</xml_diff>